<commit_message>
add filter by max_count
</commit_message>
<xml_diff>
--- a/backend/hotels.xlsx
+++ b/backend/hotels.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\hotel\hotel\backend\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\hotel\hotel\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D1F8A2E-ACCE-416A-AC94-839E00DCBF03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CDB89E1-C3A2-4B3D-9E25-E965B5EE0483}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1812" yWindow="1812" windowWidth="17256" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1816" yWindow="1816" windowWidth="17259" windowHeight="8962" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet0" sheetId="1" r:id="rId1"/>
@@ -1150,11 +1150,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -1208,7 +1208,7 @@
         <v>13</v>
       </c>
       <c r="H2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I2" t="s">
         <v>79</v>
@@ -1324,7 +1324,7 @@
         <v>13</v>
       </c>
       <c r="H6">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I6" t="s">
         <v>212</v>
@@ -1759,7 +1759,7 @@
         <v>178</v>
       </c>
       <c r="H21">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I21" t="s">
         <v>179</v>
@@ -2752,7 +2752,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I55">
+  <sortState ref="A2:I55">
     <sortCondition ref="A2:A55"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>